<commit_message>
Fix rubyXL/openpyxl format conflict
</commit_message>
<xml_diff>
--- a/data/bibliophilly_leaves-test.xlsx
+++ b/data/bibliophilly_leaves-test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emeryr/code/GIT/openn-genizah/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F86876-5C3A-E54D-946C-E4A55B6EAEE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78CC169-B208-C545-A8F3-8AC7C40200B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14660" yWindow="5720" windowWidth="26840" windowHeight="15940" xr2:uid="{7F48021B-A632-D241-9E67-C978999912AF}"/>
+    <workbookView xWindow="7660" yWindow="4080" windowWidth="26840" windowHeight="15940" xr2:uid="{4380456F-7A21-8240-8884-AEB9EB29897E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="95">
   <si>
     <t>Call Number/ID</t>
   </si>
@@ -87,6 +87,9 @@
     <t>Manuscript Name</t>
   </si>
   <si>
+    <t>Subject: Keywords</t>
+  </si>
+  <si>
     <t>Lewis E M 1:2</t>
   </si>
   <si>
@@ -120,18 +123,21 @@
     <t>Parchment</t>
   </si>
   <si>
-    <t>Latin</t>
-  </si>
-  <si>
     <t>Italy</t>
   </si>
   <si>
     <t>Lewis, John Frederick, 1860-1932</t>
   </si>
   <si>
+    <t>http://viaf.org/viaf/63874811</t>
+  </si>
+  <si>
     <t>Breviary</t>
   </si>
   <si>
+    <t>15th century|Italian|Breviary|Liturgy|Fragment</t>
+  </si>
+  <si>
     <t>Lewis E M 1:3</t>
   </si>
   <si>
@@ -150,6 +156,9 @@
     <t>Initials S, D, and F | The illumination has been attributed to the same hand that executed the decoration of the Piccolomini Gospels (New York Public Library Spencer Coll. MS 29), dated to c. 1420 or c. 1450. | These illuminated initials have been removed from the same manuscript. On the reverse are passages of text typically found in a breviary.|The illumination has been attributed to the same hand that executed the decoration of the Piccolomini Gospels (New York Public Library Spencer Coll. MS 29), dated to c. 1420 or c. 1450. | These cuttings show the reverse of four illuminated initials cut from a breviary.|</t>
   </si>
   <si>
+    <t>15th century|Italian|Italy|Breviary|Liturgy|Fragment</t>
+  </si>
+  <si>
     <t>Lewis E M 1:4</t>
   </si>
   <si>
@@ -177,6 +186,9 @@
     <t>Antiphonary</t>
   </si>
   <si>
+    <t>Antiphonary|15th century|Austria|Austrian|Liturgy|Fragment</t>
+  </si>
+  <si>
     <t>Lewis E M 1:5</t>
   </si>
   <si>
@@ -195,6 +207,9 @@
     <t>Initials E, D, and D | Rubrics on the reverse of these cuttings indicate that they were originally part of a breviary.|This image shows the reverse of two cuttings of decorated initials taken from a breviary.|</t>
   </si>
   <si>
+    <t>15th century|Breviary|Italian|Italy|Liturgy|Fragment</t>
+  </si>
+  <si>
     <t>Lewis E M 1:6</t>
   </si>
   <si>
@@ -219,6 +234,9 @@
     <t>Choir book</t>
   </si>
   <si>
+    <t>15th century|Germany|German|Song book|Musical notation|Fragment</t>
+  </si>
+  <si>
     <t>Lewis E M 1:7</t>
   </si>
   <si>
@@ -270,34 +288,28 @@
     <t>Enarrationes in psalmos (Expositions on the Psalms)</t>
   </si>
   <si>
-    <t>http://viaf.org/viaf/63874811</t>
-  </si>
-  <si>
-    <t>Former Owner name</t>
-  </si>
-  <si>
-    <t>Former Owner URI</t>
-  </si>
-  <si>
-    <t>Subject: Keywords</t>
-  </si>
-  <si>
-    <t>15th century|Italian|Breviary|Liturgy|Fragment</t>
-  </si>
-  <si>
-    <t>15th century|Italian|Italy|Breviary|Liturgy|Fragment</t>
-  </si>
-  <si>
-    <t>Antiphonary|15th century|Austria|Austrian|Liturgy|Fragment</t>
-  </si>
-  <si>
-    <t>15th century|Breviary|Italian|Italy|Liturgy|Fragment</t>
-  </si>
-  <si>
-    <t>15th century|Germany|German|Song book|Musical notation|Fragment</t>
-  </si>
-  <si>
     <t>15th century|Psalter|Bible|Biblical|Commentary|Italian|Italy|Fragment</t>
+  </si>
+  <si>
+    <t>Metadata Creator</t>
+  </si>
+  <si>
+    <t>Metadata Creator Email</t>
+  </si>
+  <si>
+    <t>David Kalish|Dot Porter</t>
+  </si>
+  <si>
+    <t>Former Owner</t>
+  </si>
+  <si>
+    <t>FO Ref</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>dexample@example.com|dorp@upenn.edu</t>
   </si>
 </sst>
 </file>
@@ -657,43 +669,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{755F9D69-14E8-1A49-9D37-315F76F800B8}">
-  <dimension ref="A1:W8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2D751B-D305-0649-A89E-D13C2CDB4257}">
+  <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1:Y1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="147.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="44.83203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -752,42 +737,48 @@
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>84</v>
+        <v>20</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J2">
         <v>1400</v>
@@ -796,16 +787,16 @@
         <v>1450</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O2" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="P2" t="s">
         <v>32</v>
@@ -814,39 +805,45 @@
         <v>33</v>
       </c>
       <c r="U2" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="V2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="W2" t="s">
-        <v>85</v>
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J3">
         <v>1400</v>
@@ -855,16 +852,16 @@
         <v>1450</v>
       </c>
       <c r="L3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O3" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="P3" t="s">
         <v>32</v>
@@ -873,39 +870,45 @@
         <v>33</v>
       </c>
       <c r="U3" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="V3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="W3" t="s">
-        <v>86</v>
+        <v>43</v>
+      </c>
+      <c r="X3" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J4">
         <v>1450</v>
@@ -914,60 +917,66 @@
         <v>1475</v>
       </c>
       <c r="L4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="M4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="N4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O4" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="P4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="T4" t="s">
         <v>33</v>
       </c>
       <c r="U4" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="V4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="W4" t="s">
-        <v>87</v>
+        <v>53</v>
+      </c>
+      <c r="X4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J5">
         <v>1400</v>
@@ -976,60 +985,66 @@
         <v>1499</v>
       </c>
       <c r="L5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="M5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="N5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O5" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="P5" t="s">
         <v>32</v>
       </c>
       <c r="Q5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="T5" t="s">
         <v>33</v>
       </c>
       <c r="U5" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="V5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="W5" t="s">
-        <v>88</v>
+        <v>60</v>
+      </c>
+      <c r="X5" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J6">
         <v>1485</v>
@@ -1038,57 +1053,63 @@
         <v>1499</v>
       </c>
       <c r="L6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="M6" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="N6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O6" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="P6" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="T6" t="s">
         <v>33</v>
       </c>
       <c r="U6" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="V6" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="W6" t="s">
-        <v>89</v>
+        <v>69</v>
+      </c>
+      <c r="X6" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J7">
         <v>1400</v>
@@ -1097,60 +1118,66 @@
         <v>1499</v>
       </c>
       <c r="L7" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="M7" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="N7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O7" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="P7" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="Q7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="T7" t="s">
         <v>33</v>
       </c>
       <c r="U7" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="V7" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="W7" t="s">
-        <v>89</v>
+        <v>69</v>
+      </c>
+      <c r="X7" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J8">
         <v>1400</v>
@@ -1159,44 +1186,53 @@
         <v>1415</v>
       </c>
       <c r="L8" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M8" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="N8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O8" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="P8" t="s">
         <v>32</v>
       </c>
       <c r="Q8" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="R8" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="S8" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="T8" t="s">
         <v>33</v>
       </c>
       <c r="U8" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="V8" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="W8" t="s">
+        <v>87</v>
+      </c>
+      <c r="X8" t="s">
         <v>90</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Y2" r:id="rId1" xr:uid="{B5073844-4716-244D-BCC0-FAA2417F706E}"/>
+    <hyperlink ref="Y3:Y8" r:id="rId2" display="dexample@example.com|dorp@upenn.edu" xr:uid="{5944EF05-4C97-DD4D-907A-5DD4FF48DDC0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>